<commit_message>
I now understand Alt1
</commit_message>
<xml_diff>
--- a/CH-142 Table Transformation.xlsx
+++ b/CH-142 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472288FC-006B-4124-BA82-3F7D74C48D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBA40FC-5BBE-45F3-8654-3D83DA9B34A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1082,6 +1082,147 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Callout: Line 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0A6AC93-0C1E-483C-9713-13E712701D40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9060180" y="2857500"/>
+          <a:ext cx="1021080" cy="388620"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout1">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 212500"/>
+            <a:gd name="adj4" fmla="val -134601"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>row number</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Callout: Line 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E20AB06F-67F0-45FB-B529-5501FC1C5F8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11010900" y="3215640"/>
+          <a:ext cx="1021080" cy="388620"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout1">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 116422"/>
+            <a:gd name="adj4" fmla="val -104750"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>2 dimensional</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t> xlookup</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1845,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD77CD4-4293-468B-9C2E-18C68F35A764}">
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Looking at my version of the line function
</commit_message>
<xml_diff>
--- a/CH-142 Table Transformation.xlsx
+++ b/CH-142 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBA40FC-5BBE-45F3-8654-3D83DA9B34A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8908FF9-4C6F-4E2F-8280-DB019E0CE236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="20">
   <si>
     <t>Result</t>
   </si>
@@ -1984,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD77CD4-4293-468B-9C2E-18C68F35A764}">
-  <dimension ref="B1:M37"/>
+  <dimension ref="B1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2423,6 +2423,7 @@
       <c r="E22" s="4">
         <v>0.46527777777777779</v>
       </c>
+      <c r="F22" s="4"/>
       <c r="G22" s="4" t="str" cm="1">
         <f t="array" ref="G22:G37">_xlfn.LET(
 _xlpm.t,E3:E18,
@@ -2485,6 +2486,7 @@
       <c r="E23" s="4">
         <v>0.73958333333333337</v>
       </c>
+      <c r="F23" s="4"/>
       <c r="G23" s="4" t="str">
         <v>Out</v>
       </c>
@@ -2520,6 +2522,7 @@
       <c r="E24" s="4">
         <v>0.70833333333333337</v>
       </c>
+      <c r="F24" s="4"/>
       <c r="G24" s="4" t="str">
         <v>In</v>
       </c>
@@ -2555,6 +2558,7 @@
       <c r="E25" s="4">
         <v>0.70833333333333337</v>
       </c>
+      <c r="F25" s="4"/>
       <c r="G25" s="4" t="str">
         <v>Out</v>
       </c>
@@ -2590,6 +2594,7 @@
       <c r="E26" s="4">
         <v>0.70833333333333337</v>
       </c>
+      <c r="F26" s="4"/>
       <c r="G26" s="4" t="str">
         <v>In</v>
       </c>
@@ -2625,6 +2630,7 @@
       <c r="E27" s="4">
         <v>0.42708333333333331</v>
       </c>
+      <c r="F27" s="4"/>
       <c r="G27" s="4" t="str">
         <v>Out</v>
       </c>
@@ -2660,6 +2666,7 @@
       <c r="E28" s="4">
         <v>0.59375</v>
       </c>
+      <c r="F28" s="4"/>
       <c r="G28" s="4" t="str">
         <v>In</v>
       </c>
@@ -2695,6 +2702,7 @@
       <c r="E29" s="4" t="str">
         <v/>
       </c>
+      <c r="F29" s="4"/>
       <c r="G29" s="4" t="str">
         <v>Out</v>
       </c>
@@ -2730,6 +2738,7 @@
       <c r="E30" s="4" t="str">
         <v/>
       </c>
+      <c r="F30" s="4"/>
       <c r="G30" s="4" t="str">
         <v>In</v>
       </c>
@@ -2765,6 +2774,7 @@
       <c r="E31" s="4" t="str">
         <v/>
       </c>
+      <c r="F31" s="4"/>
       <c r="G31" s="4" t="str">
         <v>Out</v>
       </c>
@@ -2788,6 +2798,7 @@
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F32" s="4"/>
       <c r="G32" s="4" t="str">
         <v>In</v>
       </c>
@@ -2798,7 +2809,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F33" s="4"/>
       <c r="G33" s="4" t="str">
         <v>Out</v>
       </c>
@@ -2809,7 +2821,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="4">
+        <v>1</v>
+      </c>
       <c r="G34" s="4" t="str">
         <v>Out</v>
       </c>
@@ -2820,7 +2841,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="4">
+        <v>1</v>
+      </c>
       <c r="G35" s="4" t="str">
         <v>In</v>
       </c>
@@ -2831,7 +2861,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2</v>
+      </c>
       <c r="G36" s="4" t="str">
         <v>In</v>
       </c>
@@ -2842,7 +2881,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="4">
+        <v>2</v>
+      </c>
       <c r="G37" s="4" t="str">
         <v>In</v>
       </c>
@@ -2851,6 +2899,132 @@
       </c>
       <c r="I37" s="4">
         <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made my own function
</commit_message>
<xml_diff>
--- a/CH-142 Table Transformation.xlsx
+++ b/CH-142 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8908FF9-4C6F-4E2F-8280-DB019E0CE236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148972CA-E4EF-41A3-AA3D-6DF4B2B565D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="22">
   <si>
     <t>Result</t>
   </si>
@@ -132,12 +132,18 @@
   <si>
     <t>t</t>
   </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +185,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -462,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -593,6 +605,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1531,7 +1546,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="873" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1984,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD77CD4-4293-468B-9C2E-18C68F35A764}">
-  <dimension ref="B1:M49"/>
+  <dimension ref="B1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1997,7 +2012,8 @@
     <col min="3" max="5" width="6.69921875" style="4" customWidth="1"/>
     <col min="6" max="6" width="45.19921875" style="5" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="10" width="6.69921875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="6.69921875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="13.296875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2809,7 +2825,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C33" s="45" t="s">
+        <v>8</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4" t="str">
         <v>Out</v>
@@ -2821,7 +2840,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C34" s="4" t="s">
         <v>7</v>
       </c>
@@ -2829,6 +2851,9 @@
         <v>8</v>
       </c>
       <c r="E34" s="4">
+        <v>1</v>
+      </c>
+      <c r="F34" s="5">
         <v>1</v>
       </c>
       <c r="G34" s="4" t="str">
@@ -2841,7 +2866,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C35" s="4" t="s">
         <v>8</v>
       </c>
@@ -2850,6 +2878,9 @@
       </c>
       <c r="E35" s="4">
         <v>1</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0</v>
       </c>
       <c r="G35" s="4" t="str">
         <v>In</v>
@@ -2861,7 +2892,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C36" s="4" t="s">
         <v>7</v>
       </c>
@@ -2871,6 +2905,9 @@
       <c r="E36" s="4">
         <v>2</v>
       </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
       <c r="G36" s="4" t="str">
         <v>In</v>
       </c>
@@ -2881,7 +2918,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C37" s="4" t="s">
         <v>8</v>
       </c>
@@ -2891,6 +2931,9 @@
       <c r="E37" s="4">
         <v>2</v>
       </c>
+      <c r="F37" s="5">
+        <v>0</v>
+      </c>
       <c r="G37" s="4" t="str">
         <v>In</v>
       </c>
@@ -2901,7 +2944,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C38" s="4" t="s">
         <v>7</v>
       </c>
@@ -2911,8 +2957,14 @@
       <c r="E38" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F38" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>8</v>
       </c>
@@ -2922,8 +2974,14 @@
       <c r="E39" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C40" s="4" t="s">
         <v>7</v>
       </c>
@@ -2933,8 +2991,14 @@
       <c r="E40" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C41" s="4" t="s">
         <v>8</v>
       </c>
@@ -2944,8 +3008,40 @@
       <c r="E41" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F41" s="5">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4" cm="1">
+        <f t="array" ref="G41:G55">_xlfn.SCAN(,F34:F48,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v))</f>
+        <v>1</v>
+      </c>
+      <c r="J41" s="27" cm="1">
+        <f t="array" ref="J41:M50">_xlfn.LET(
+_xlpm.d,E3:E18,
+_xlpm.q,_xlfn.SCAN("Out|0",_xlpm.d,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.v&amp;"|"&amp;IF(AND(_xlpm.v&lt;&gt;"In",_xlfn.TEXTBEFORE(_xlpm.a,"|")&lt;&gt;"Out"),1,0))),
+_xlpm.qq,1-_xlfn.DROP(_xlfn.REDUCE(0,_xlpm.q,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTAFTER(_xlpm.v,"|")))),1),
+_xlpm.qqq, _xlfn.SCAN(,_xlpm.qq,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v)),
+_xlpm.qqqq,_xlfn.HSTACK(
+        _xlfn._xlws.FILTER(B3:C18, _xlpm.qq),
+        _xlfn.XLOOKUP(_xlfn.UNIQUE(_xlpm.qqq) &amp; {"In","Out"}, _xlpm.qqq &amp; E3:E18, D3:D18, "")    ),
+_xlpm.qqqq
+)</f>
+        <v>45584</v>
+      </c>
+      <c r="K41" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="L41" s="28">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M41" s="24">
+        <v>0.46527777777777779</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C42" s="4" t="s">
         <v>7</v>
       </c>
@@ -2955,8 +3051,29 @@
       <c r="E42" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F42" s="5">
+        <v>1</v>
+      </c>
+      <c r="G42" s="4">
+        <v>1</v>
+      </c>
+      <c r="J42" s="27">
+        <v>45584</v>
+      </c>
+      <c r="K42" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="L42" s="28">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="M42" s="24">
+        <v>0.73958333333333337</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C43" s="4" t="s">
         <v>8</v>
       </c>
@@ -2966,8 +3083,29 @@
       <c r="E43" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F43" s="5">
+        <v>0</v>
+      </c>
+      <c r="G43" s="4">
+        <v>2</v>
+      </c>
+      <c r="J43" s="10">
+        <v>45584</v>
+      </c>
+      <c r="K43" s="11" t="str">
+        <v>B</v>
+      </c>
+      <c r="L43" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M43" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C44" s="4" t="s">
         <v>7</v>
       </c>
@@ -2977,8 +3115,29 @@
       <c r="E44" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F44" s="5">
+        <v>1</v>
+      </c>
+      <c r="G44" s="4">
+        <v>2</v>
+      </c>
+      <c r="J44" s="10">
+        <v>45585</v>
+      </c>
+      <c r="K44" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="L44" s="12">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="M44" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C45" s="4" t="s">
         <v>8</v>
       </c>
@@ -2988,8 +3147,29 @@
       <c r="E45" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F45" s="5">
+        <v>1</v>
+      </c>
+      <c r="G45" s="4">
+        <v>3</v>
+      </c>
+      <c r="J45" s="10">
+        <v>45585</v>
+      </c>
+      <c r="K45" s="11" t="str">
+        <v>B</v>
+      </c>
+      <c r="L45" s="12">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="M45" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C46" s="4" t="s">
         <v>8</v>
       </c>
@@ -2999,8 +3179,29 @@
       <c r="E46" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F46" s="5">
+        <v>1</v>
+      </c>
+      <c r="G46" s="4">
+        <v>3</v>
+      </c>
+      <c r="J46" s="10">
+        <v>45586</v>
+      </c>
+      <c r="K46" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="L46" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M46" s="13">
+        <v>0.42708333333333331</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C47" s="4" t="s">
         <v>7</v>
       </c>
@@ -3010,8 +3211,29 @@
       <c r="E47" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F47" s="5">
+        <v>1</v>
+      </c>
+      <c r="G47" s="4">
+        <v>4</v>
+      </c>
+      <c r="J47" s="10">
+        <v>45586</v>
+      </c>
+      <c r="K47" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="L47" s="14" t="str">
+        <v/>
+      </c>
+      <c r="M47" s="13">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C48" s="4" t="s">
         <v>7</v>
       </c>
@@ -3021,10 +3243,85 @@
       <c r="E48" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="4" t="s">
-        <v>7</v>
+      <c r="F48" s="5">
+        <v>1</v>
+      </c>
+      <c r="G48" s="4">
+        <v>4</v>
+      </c>
+      <c r="J48" s="10">
+        <v>45586</v>
+      </c>
+      <c r="K48" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="L48" s="12">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="M48" s="11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="4">
+        <v>5</v>
+      </c>
+      <c r="J49" s="10">
+        <v>45587</v>
+      </c>
+      <c r="K49" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="L49" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M49" s="13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G50" s="4">
+        <v>5</v>
+      </c>
+      <c r="J50" s="10">
+        <v>45587</v>
+      </c>
+      <c r="K50" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="L50" s="12">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="M50" s="13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G51" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G52" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G53" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G54" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G55" s="4">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>